<commit_message>
updated at entry functions
</commit_message>
<xml_diff>
--- a/Dbschema.xlsx
+++ b/Dbschema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\COVIDSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E139B860-DA26-4C82-82A6-48DC9323CBE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFA009B-D5C3-4BD3-8E61-BDCB3509F063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
   <si>
     <t>Nurse:</t>
   </si>
@@ -177,21 +177,12 @@
     <t>P_ward</t>
   </si>
   <si>
-    <t>P_bedNo</t>
-  </si>
-  <si>
-    <t>LONG</t>
-  </si>
-  <si>
     <t>VARCHAR(1)</t>
   </si>
   <si>
     <t>P_bg</t>
   </si>
   <si>
-    <t>VARCHAR2(2)</t>
-  </si>
-  <si>
     <t>P_temp</t>
   </si>
   <si>
@@ -201,9 +192,6 @@
     <t>P_O2Level</t>
   </si>
   <si>
-    <t>VARCHAR2(10)</t>
-  </si>
-  <si>
     <t>P_covlevel</t>
   </si>
   <si>
@@ -216,21 +204,9 @@
     <t>REC_NO</t>
   </si>
   <si>
-    <t>NUMBER</t>
-  </si>
-  <si>
     <t>W_type</t>
   </si>
   <si>
-    <t>NoOfBeds_Full</t>
-  </si>
-  <si>
-    <t>WardCapacity</t>
-  </si>
-  <si>
-    <t>W_NAME</t>
-  </si>
-  <si>
     <t>Nurse1</t>
   </si>
   <si>
@@ -243,9 +219,6 @@
     <t>Wardboy2</t>
   </si>
   <si>
-    <t>Doctor</t>
-  </si>
-  <si>
     <t>N_add_date</t>
   </si>
   <si>
@@ -253,6 +226,24 @@
   </si>
   <si>
     <t>D_add_date</t>
+  </si>
+  <si>
+    <t>WARDNAME</t>
+  </si>
+  <si>
+    <t>Doctor1</t>
+  </si>
+  <si>
+    <t>No_Of_Beds_Full</t>
+  </si>
+  <si>
+    <t>W_Capacity</t>
+  </si>
+  <si>
+    <t>VARCHAR2(15)</t>
+  </si>
+  <si>
+    <t>VARCHAR2(4)</t>
   </si>
 </sst>
 </file>
@@ -296,7 +287,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -323,10 +314,34 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -336,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -350,9 +365,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -668,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672780C-ACB8-45C8-8FBA-C47A5E0920AC}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -680,31 +707,31 @@
     <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.109375" customWidth="1"/>
     <col min="4" max="4" width="3.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.21875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.109375" customWidth="1"/>
     <col min="7" max="7" width="16.44140625" customWidth="1"/>
     <col min="8" max="8" width="3.33203125" customWidth="1"/>
-    <col min="9" max="9" width="11.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.77734375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.21875" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="E1" s="8" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="E1" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="I1" s="8" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="I1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -987,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>43</v>
@@ -996,36 +1023,47 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="G12" s="6"/>
     </row>
+    <row r="13" spans="1:11">
+      <c r="I13" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="10"/>
+    </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="E14" s="8" t="s">
+      <c r="A14" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="E14" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="I14" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" s="2" t="s">
@@ -1046,14 +1084,14 @@
       <c r="G15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>3</v>
+      <c r="I15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -1070,19 +1108,19 @@
         <v>67</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>52</v>
+        <v>14</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="K16" s="4" t="s">
-        <v>19</v>
+        <v>39</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1096,22 +1134,22 @@
         <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>20</v>
+        <v>72</v>
+      </c>
+      <c r="K17" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1125,7 +1163,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>14</v>
@@ -1134,10 +1172,10 @@
         <v>17</v>
       </c>
       <c r="I18" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>17</v>
@@ -1154,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>14</v>
@@ -1163,10 +1201,10 @@
         <v>17</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="K19" s="4" t="s">
         <v>17</v>
@@ -1183,17 +1221,17 @@
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>17</v>
@@ -1204,23 +1242,23 @@
         <v>48</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="4"/>
       <c r="I21" s="4" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>58</v>
+        <v>16</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>17</v>
@@ -1237,34 +1275,28 @@
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6" t="s">
         <v>49</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -1272,17 +1304,15 @@
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="7" t="s">
-        <v>50</v>
+      <c r="A24" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>20</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C24" s="4"/>
       <c r="E24" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -1291,30 +1321,21 @@
     </row>
     <row r="25" spans="1:11">
       <c r="A25" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C25" s="4"/>
     </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="I13:K13"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="E14:G14"/>
-    <mergeCell ref="I14:K14"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated nurse functionalities and added isexist()
</commit_message>
<xml_diff>
--- a/Dbschema.xlsx
+++ b/Dbschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\COVIDSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFA009B-D5C3-4BD3-8E61-BDCB3509F063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3999A17-7093-4FB6-BD41-C546983ED90D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
+    <workbookView xWindow="9516" yWindow="1956" windowWidth="13524" windowHeight="9612" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,8 +365,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -377,9 +378,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -697,8 +697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672780C-ACB8-45C8-8FBA-C47A5E0920AC}">
   <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -717,21 +717,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="E1" s="7" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="I1" s="7" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -1038,23 +1038,23 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="9"/>
-      <c r="K13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="E14" s="7" t="s">
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
       <c r="I14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1281,9 +1281,9 @@
         <v>5</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="11"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6" t="s">

</xml_diff>

<commit_message>
updated schema with addition of new columns
</commit_message>
<xml_diff>
--- a/Dbschema.xlsx
+++ b/Dbschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\COVIDSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A87A192-11E8-4085-8813-DF47A162B8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DEB1C6-708B-41D4-A933-E15E01B16C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9516" yWindow="1956" windowWidth="13524" windowHeight="9612" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
   <si>
     <t>Nurse:</t>
   </si>
@@ -198,9 +198,6 @@
     <t>Patient_phys:</t>
   </si>
   <si>
-    <t>Patient_at_Rec:</t>
-  </si>
-  <si>
     <t>REC_NO</t>
   </si>
   <si>
@@ -244,6 +241,12 @@
   </si>
   <si>
     <t>VARCHAR2(4)</t>
+  </si>
+  <si>
+    <t>P_add_date</t>
+  </si>
+  <si>
+    <t>Patient_at_entry:</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -365,10 +368,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -695,10 +694,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672780C-ACB8-45C8-8FBA-C47A5E0920AC}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -717,21 +716,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="E1" s="12" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="E1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="I1" s="12" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="I1" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -1014,7 +1013,7 @@
         <v>20</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>43</v>
@@ -1023,14 +1022,14 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>43</v>
@@ -1038,23 +1037,23 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="11"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="9"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="E14" s="12" t="s">
+      <c r="A14" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="E14" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
       <c r="I14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1085,7 +1084,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>14</v>
@@ -1105,7 +1104,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>14</v>
@@ -1134,7 +1133,7 @@
         <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>50</v>
@@ -1146,7 +1145,7 @@
         <v>51</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>17</v>
@@ -1163,7 +1162,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>14</v>
@@ -1192,7 +1191,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>14</v>
@@ -1221,7 +1220,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
@@ -1242,23 +1241,23 @@
         <v>48</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>45</v>
+      <c r="I21" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>17</v>
@@ -1275,15 +1274,12 @@
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="4"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6" t="s">
@@ -1296,7 +1292,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -1312,7 +1308,7 @@
       </c>
       <c r="C24" s="4"/>
       <c r="E24" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -1327,6 +1323,17 @@
         <v>43</v>
       </c>
       <c r="C25" s="4"/>
+    </row>
+    <row r="26" spans="1:11">
+      <c r="A26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Revert "Merge branch 'main' of https://github.com/Abhishek-Kamble/COVID-Java-SQL into main"
This reverts commit 277a0a5f5eaa0d5c609332ab8182185112a80507, reversing
changes made to ed0a89fb48e27fb07ac3dd322513c1f12aa0e809.
</commit_message>
<xml_diff>
--- a/Dbschema.xlsx
+++ b/Dbschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\COVIDSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5DEB1C6-708B-41D4-A933-E15E01B16C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A87A192-11E8-4085-8813-DF47A162B8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
+    <workbookView xWindow="9516" yWindow="1956" windowWidth="13524" windowHeight="9612" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
   <si>
     <t>Nurse:</t>
   </si>
@@ -198,6 +198,9 @@
     <t>Patient_phys:</t>
   </si>
   <si>
+    <t>Patient_at_Rec:</t>
+  </si>
+  <si>
     <t>REC_NO</t>
   </si>
   <si>
@@ -241,12 +244,6 @@
   </si>
   <si>
     <t>VARCHAR2(4)</t>
-  </si>
-  <si>
-    <t>P_add_date</t>
-  </si>
-  <si>
-    <t>Patient_at_entry:</t>
   </si>
 </sst>
 </file>
@@ -354,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -368,6 +365,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672780C-ACB8-45C8-8FBA-C47A5E0920AC}">
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -716,21 +717,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="E1" s="10" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="E1" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="I1" s="10" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="I1" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="2" t="s">
@@ -1013,7 +1014,7 @@
         <v>20</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J11" s="5" t="s">
         <v>43</v>
@@ -1022,14 +1023,14 @@
     </row>
     <row r="12" spans="1:11">
       <c r="A12" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C12" s="6"/>
       <c r="E12" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="F12" s="5" t="s">
         <v>43</v>
@@ -1037,23 +1038,23 @@
       <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:11">
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11">
-      <c r="A14" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="E14" s="10" t="s">
+      <c r="A14" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="E14" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
       <c r="I14" s="2" t="s">
         <v>1</v>
       </c>
@@ -1084,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J15" s="4" t="s">
         <v>14</v>
@@ -1104,7 +1105,7 @@
         <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>14</v>
@@ -1133,7 +1134,7 @@
         <v>17</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>50</v>
@@ -1145,7 +1146,7 @@
         <v>51</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>17</v>
@@ -1162,7 +1163,7 @@
         <v>17</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>14</v>
@@ -1191,7 +1192,7 @@
         <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F19" s="5" t="s">
         <v>14</v>
@@ -1220,7 +1221,7 @@
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
@@ -1241,23 +1242,23 @@
         <v>48</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="I21" s="6" t="s">
-        <v>72</v>
+      <c r="I21" s="4" t="s">
+        <v>45</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>43</v>
+        <v>16</v>
       </c>
       <c r="K21" s="4" t="s">
         <v>17</v>
@@ -1274,12 +1275,15 @@
         <v>17</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F22" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G22" s="4"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="7"/>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" s="6" t="s">
@@ -1292,7 +1296,7 @@
         <v>20</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F23" s="5" t="s">
         <v>5</v>
@@ -1308,7 +1312,7 @@
       </c>
       <c r="C24" s="4"/>
       <c r="E24" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F24" s="5" t="s">
         <v>5</v>
@@ -1323,17 +1327,6 @@
         <v>43</v>
       </c>
       <c r="C25" s="4"/>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>17</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>

<commit_message>
Updated scheama by rem columns
</commit_message>
<xml_diff>
--- a/Dbschema.xlsx
+++ b/Dbschema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eclipse\COVIDSQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A87A192-11E8-4085-8813-DF47A162B8F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23C66B56-C6FD-4B7D-B237-08FE9A97B4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9516" yWindow="1956" windowWidth="13524" windowHeight="9612" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{DA7FB309-F4A1-4205-B036-B3F21EAB7F7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="68">
   <si>
     <t>Nurse:</t>
   </si>
@@ -81,9 +81,6 @@
     <t>NOT NULL</t>
   </si>
   <si>
-    <t>N_ward</t>
-  </si>
-  <si>
     <t>PRIMARY KEY</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>D_status</t>
   </si>
   <si>
-    <t>D_ward</t>
-  </si>
-  <si>
     <t>Doctor:</t>
   </si>
   <si>
@@ -138,9 +132,6 @@
     <t>W_status</t>
   </si>
   <si>
-    <t>W_ward</t>
-  </si>
-  <si>
     <t>Ward:</t>
   </si>
   <si>
@@ -210,13 +201,7 @@
     <t>Nurse1</t>
   </si>
   <si>
-    <t>Nurse2</t>
-  </si>
-  <si>
     <t>Wardboy1</t>
-  </si>
-  <si>
-    <t>Wardboy2</t>
   </si>
   <si>
     <t>N_add_date</t>
@@ -695,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3672780C-ACB8-45C8-8FBA-C47A5E0920AC}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -723,12 +708,12 @@
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
       <c r="E1" s="12" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" s="12"/>
       <c r="G1" s="12"/>
       <c r="I1" s="12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J1" s="12"/>
       <c r="K1" s="12"/>
@@ -770,25 +755,25 @@
         <v>5</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J3" s="5" t="s">
         <v>5</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -802,7 +787,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>7</v>
@@ -811,7 +796,7 @@
         <v>17</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J4" s="5" t="s">
         <v>7</v>
@@ -831,7 +816,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>14</v>
@@ -840,7 +825,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J5" s="5" t="s">
         <v>14</v>
@@ -860,7 +845,7 @@
         <v>17</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>5</v>
@@ -869,7 +854,7 @@
         <v>17</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J6" s="5" t="s">
         <v>5</v>
@@ -889,7 +874,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>15</v>
@@ -898,7 +883,7 @@
         <v>17</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J7" s="5" t="s">
         <v>15</v>
@@ -918,7 +903,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>7</v>
@@ -956,7 +941,7 @@
         <v>17</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="J9" s="5" t="s">
         <v>16</v>
@@ -976,7 +961,7 @@
         <v>17</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>16</v>
@@ -985,112 +970,112 @@
         <v>17</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>37</v>
+        <v>60</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11">
       <c r="A11" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="E11" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="6"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="I12" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="11"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="E13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="E12" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" s="6"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="I13" s="9" t="s">
-        <v>56</v>
-      </c>
-      <c r="J13" s="10"/>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="E14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="I14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>3</v>
+      <c r="A15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="K15" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1099,54 +1084,54 @@
         <v>39</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K16" s="6" t="s">
-        <v>20</v>
+      <c r="K16" s="4" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="4" t="s">
-        <v>59</v>
+      <c r="E17" s="6" t="s">
+        <v>65</v>
       </c>
       <c r="F17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="K17" s="4" t="s">
         <v>17</v>
@@ -1154,16 +1139,16 @@
     </row>
     <row r="18" spans="1:11">
       <c r="A18" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>70</v>
+      <c r="E18" s="4" t="s">
+        <v>64</v>
       </c>
       <c r="F18" s="5" t="s">
         <v>14</v>
@@ -1172,10 +1157,10 @@
         <v>17</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>53</v>
+        <v>14</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>17</v>
@@ -1183,25 +1168,23 @@
     </row>
     <row r="19" spans="1:11">
       <c r="A19" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="G19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>14</v>
@@ -1212,26 +1195,26 @@
     </row>
     <row r="20" spans="1:11">
       <c r="A20" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G20" s="4"/>
       <c r="I20" s="4" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>17</v>
@@ -1239,103 +1222,62 @@
     </row>
     <row r="21" spans="1:11">
       <c r="A21" s="4" t="s">
-        <v>48</v>
+        <v>12</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>71</v>
+        <v>16</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="4" t="s">
-        <v>61</v>
+      <c r="E21" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>5</v>
       </c>
       <c r="G21" s="4"/>
-      <c r="I21" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="K21" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="7"/>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="4" t="s">
-        <v>12</v>
+      <c r="A22" s="6" t="s">
+        <v>46</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G22" s="4"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="6" t="s">
-        <v>49</v>
+      <c r="A23" s="4" t="s">
+        <v>37</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G23" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:11">
       <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="C24" s="4"/>
-      <c r="E24" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G24" s="4"/>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C25" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="I13:K13"/>
+    <mergeCell ref="I12:K12"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="I1:K1"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="E14:G14"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="E13:G13"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>